<commit_message>
Updated during 2019-09-20 call
added further detail for specifying codelist variable
</commit_message>
<xml_diff>
--- a/WorkingDocs/03a_DB Specs - Input.xlsx
+++ b/WorkingDocs/03a_DB Specs - Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\omseafile01.omeros.local\users\dditommaso\documents\SP\PhUSE\TDF_Material\WorkingDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2BBC2C-A236-49B6-8076-00DA00C035BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F5B3DA-9AAE-4EFB-BB7C-4C75D3531BA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37740" yWindow="1620" windowWidth="19710" windowHeight="13935" activeTab="1" xr2:uid="{880C47D5-0322-439C-976E-C01FC6A3EC9D}"/>
+    <workbookView xWindow="21660" yWindow="-4125" windowWidth="21600" windowHeight="13575" xr2:uid="{880C47D5-0322-439C-976E-C01FC6A3EC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable Modeling" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -261,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="324">
   <si>
     <t>DM – Specification</t>
   </si>
@@ -1259,6 +1260,9 @@
   <si>
     <t>[YYYY-MM-DDThh:mm|YYYY-MM-DDThh:mm), or
 TDM (GSK) metadata?</t>
+  </si>
+  <si>
+    <t>codelist(ct-id, term-weight-list|dset)</t>
   </si>
 </sst>
 </file>
@@ -1802,7 +1806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2D4D11-0CDE-4425-AE04-397E11022DFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1841,7 +1847,9 @@
       <c r="B2" t="s">
         <v>286</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="20" t="s">
+        <v>323</v>
+      </c>
       <c r="D2" s="21" t="s">
         <v>291</v>
       </c>
@@ -1996,7 +2004,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>